<commit_message>
Message décrivant la modification
</commit_message>
<xml_diff>
--- a/Revue_Litterature/Revue_Littéraire.xlsx
+++ b/Revue_Litterature/Revue_Littéraire.xlsx
@@ -5,15 +5,16 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AS2_2024-2025\Semestre 2\Rapport_Stage_2024_2025_Cheikh_Oumar_SAKHO\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\AS2_2024-2025\Semestre 2\Rapport_Stage_2024_2025_Cheikh_Oumar_SAKHO\Revue_Litterature\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5840B173-E1E3-4DAA-BB7B-3A1725D0E9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A910BAE6-5915-41AF-AF51-D0954F99F23A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" xr2:uid="{6D4C1247-2136-4D77-9A13-954005E84CCF}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="22695" windowHeight="14476" activeTab="1" xr2:uid="{6D4C1247-2136-4D77-9A13-954005E84CCF}"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
+    <sheet name="Feuil2" sheetId="2" r:id="rId2"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="64" uniqueCount="64">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="139">
   <si>
     <t>Titre de l’article</t>
   </si>
@@ -229,12 +230,237 @@
   <si>
     <t>- Étude limitée à Ouagadougou (1 498 ménages)- Attribution arbitraire des scores aux modalités- Faible corrélation des proxys avec l'indicateur de référence- Nécessité de validation sur d'autres contextes géographiques</t>
   </si>
+  <si>
+    <t>Titre de l'article</t>
+  </si>
+  <si>
+    <t>Quatre profils de quartiers identifiés selon la qualité du logement ; le profil avec la plus faible qualité présente un taux de mortalité significativement plus élevé. La qualité du logement est un facteur de risque important pour la santé.</t>
+  </si>
+  <si>
+    <t>Qualité du logement (confort, matériaux, accès à l'eau, planification urbaine), environnement végétalisé, propriétés de faible qualité, zones d'affaires</t>
+  </si>
+  <si>
+    <t>16 variables : propriété, type de toit, type de murs, revêtement de sol, système d'égouts, robinet privé, habitat planifié/défavorisé, densité de population, végétation, sol nu, etc.</t>
+  </si>
+  <si>
+    <t>Recensement 2013, données satellite 2015</t>
+  </si>
+  <si>
+    <t>Taux de mortalité brut non ajusté à l'âge, risque de sous-déclaration des décès, agrégation au niveau du quartier (erreur écologique), décalage temporel entre sources</t>
+  </si>
+  <si>
+    <t>Extension de la méthode SPREE (Structure Preserving Estimation) intégrant données auxiliaires (imagerie satellite) pour actualiser les indicateurs de pauvreté multidimensionnelle à petite échelle</t>
+  </si>
+  <si>
+    <t>L'imagerie satellite améliore la précision des estimations de population, surtout dans zones à grands changements démographiques. Mises à jour annuelles de la pauvreté multidimensionnelle pour communes du Sénégal 2013-2020.</t>
+  </si>
+  <si>
+    <t>Statut de pauvreté, sexe du chef de ménage, mortalité infantile, scolarité, combustible de cuisson, assainissement, eau potable, électricité, logement, actifs</t>
+  </si>
+  <si>
+    <t>Qualité limitée des données satellitaires pour certaines zones, incertitude difficile à quantifier, définitions variables selon sources, impossibilité d'évaluer directement au niveau communal après 2013</t>
+  </si>
+  <si>
+    <t>Non spécifiée</t>
+  </si>
+  <si>
+    <t>African Population Studies Supplement A to vol 19</t>
+  </si>
+  <si>
+    <t>Comparaison de 4 méthodes d'agrégation : sommation simple, standardisation IDH, Analyse en Composantes Principales (ACP), Analyse des Correspondances Multiples (ACM) + ACP</t>
+  </si>
+  <si>
+    <t>Proxys habitat/biens faiblement corrélés à l'indicateur dépenses (r ≤ 0,37). L'indicateur dépenses rend mieux compte des inégalités de scolarisation. Forte corrélation entre proxys (r ≥ 0,95)</t>
+  </si>
+  <si>
+    <t>Habitat : murs, sols, aisances, douche, ordures, pièces, eau, énergie. Biens : déplacement, TV, radio, réfrigérateur, téléphone</t>
+  </si>
+  <si>
+    <t>Enquête DSA 1994-95 (Burkina Faso)</t>
+  </si>
+  <si>
+    <t>Étude limitée à Ouagadougou (1 498 ménages), attribution arbitraire des scores, faible corrélation avec indicateur de référence, nécessité de validation géographique</t>
+  </si>
+  <si>
+    <t>Guide méthodologique sur le repérage de l'habitat indigne – Les actions de repérage : mode d'emploi</t>
+  </si>
+  <si>
+    <t>Bruno Desaubliaux (responsable), Philippe Payet, Muriel Casalis</t>
+  </si>
+  <si>
+    <t>CETE Méditerranée - Délégation interministérielle à l'hébergement et à l'accès au logement (DIHAL)</t>
+  </si>
+  <si>
+    <t>Exploitation statistique (FILOCOM, MAJIC3, fichiers fonciers), pré-repérage PPPI, analyse factorielle, croisement avec enquêtes terrain</t>
+  </si>
+  <si>
+    <t>Identification des logements potentiellement indignes, mise en évidence des facteurs de dégradation, outils pour définir priorités territoriales et politiques de prévention</t>
+  </si>
+  <si>
+    <t>Type de logement, nombre de pièces, surface, année de construction, statut d'occupation, durée de vacance, revenus des ménages, situation familiale, mutations immobilières</t>
+  </si>
+  <si>
+    <t>Accès restreint aux données fiscales, ne remplace pas le terrain, pas d'évaluations comparatives nationales, dépendance qualité sources fiscales, contraintes secret statistique, temporalité des fichiers</t>
+  </si>
+  <si>
+    <t>Chapitre 10 dans "Crise et population en Afrique" (ORSTOM)</t>
+  </si>
+  <si>
+    <t>Analyse comparative recensements/enquêtes sur deux villes (Abidjan et Dakar), analyse diachronique (1960-1990), typologie de l'habitat</t>
+  </si>
+  <si>
+    <t>Ralentissement croissance urbaine années 1980, densification quartiers centraux, augmentation locataires, retard accès au logement jeunes générations, diversification modes d'occupation</t>
+  </si>
+  <si>
+    <t>Types d'habitat (résidentiel, économique, évolutif, spontané), statut d'occupation, caractéristiques démographiques, accès aux équipements</t>
+  </si>
+  <si>
+    <t>Densité d'occupation, taille ménages, proportion propriétaires/locataires, âge d'accès au logement, revenus par habitat, taux d'accès réseaux, prix des loyers</t>
+  </si>
+  <si>
+    <t>1955-1989 (focus 1970-1980)</t>
+  </si>
+  <si>
+    <t>Manque de données fines comparatives, difficultés à isoler effets crise des tendances structurelles, données ponctuelles, ambiguïtés typologies, confusion ménage/logement</t>
+  </si>
+  <si>
+    <t>Document PDF : 010008009.pdf</t>
+  </si>
+  <si>
+    <t>La politique de l'habitat au Sénégal : une mutation permanente</t>
+  </si>
+  <si>
+    <t>Youssouph Sané</t>
+  </si>
+  <si>
+    <t>Les Cahiers d'Outre-Mer, n° 263</t>
+  </si>
+  <si>
+    <t>Analyse historique et politique diachronique (1862-2013) des politiques d'habitat et d'urbanisme</t>
+  </si>
+  <si>
+    <t>Evolution des politiques : de "déguerpissement" colonial vers restructuration participative ; 67,2% propriétaires vs 19,1% locataires (2002) ; loyer moyen 56 000 FCFA/mois (2009) ; besoin estimé 100 000-200 000 logements/an</t>
+  </si>
+  <si>
+    <t>Politique publique, Evolution historique, Typologie d'habitat, Financement, Restructuration urbaine</t>
+  </si>
+  <si>
+    <t>Statut d'occupation, types d'habitat, prix des loyers, démographie urbaine, mécanismes de financement (SICAP, SNHLM, BHS, FORREF), programmes (parcelles assainies, ZAC, coopératives)</t>
+  </si>
+  <si>
+    <t>Focus géographique sur Dakar, analyse historique plutôt que méthodologique pour construction d'indicateurs, données fragmentées selon les périodes</t>
+  </si>
+  <si>
+    <t>https://journals.openedition.org/com/6913</t>
+  </si>
+  <si>
+    <t>Rapports du RGPHAE 2013 : Habitat</t>
+  </si>
+  <si>
+    <t>ANSD - Agence Nationale de la Statistique et de la Démographie</t>
+  </si>
+  <si>
+    <t>ANSD Sénégal</t>
+  </si>
+  <si>
+    <t>Recensement national</t>
+  </si>
+  <si>
+    <t>Données statistiques nationales sur l'habitat : 74,7% des habitations avec revêtement en ciment, 57,5% accès à l'électricité</t>
+  </si>
+  <si>
+    <t>Infrastructure, Equipements de base, Matériaux de construction</t>
+  </si>
+  <si>
+    <t>Revêtement des habitations, source d'énergie pour l'éclairage, accès aux services</t>
+  </si>
+  <si>
+    <t>Données descriptives sans construction d'indicateurs composites</t>
+  </si>
+  <si>
+    <t>https://www.ansd.sn/Indicateur/rapports-du-rgphae-2013-habitat-0</t>
+  </si>
+  <si>
+    <t>Indice du Coût de la Construction (ICC) base 100 2018</t>
+  </si>
+  <si>
+    <t>Indice de Laspeyres</t>
+  </si>
+  <si>
+    <t>Construction d'un indice composite du coût de la construction par zones écologiques/économiques</t>
+  </si>
+  <si>
+    <t>Coût de construction, Variations temporelles, Zonage géographique</t>
+  </si>
+  <si>
+    <t>Prix des matériaux, coût de la main d'œuvre, types de logement représentatifs</t>
+  </si>
+  <si>
+    <t>Focalisé sur les coûts, pas sur la qualité ou l'accès à l'habitat</t>
+  </si>
+  <si>
+    <t>https://www.ansd.sn/Indicateur/indice-du-cout-de-la-construction-icc-base-100-2018</t>
+  </si>
+  <si>
+    <t>Indice du Chiffre d'Affaires dans la Construction (ICAC)</t>
+  </si>
+  <si>
+    <t>Année à préciser</t>
+  </si>
+  <si>
+    <t>Indice sectoriel</t>
+  </si>
+  <si>
+    <t>Suivi de l'activité de construction (bâtiments, infrastructures) selon CITI rev4/NAEMA rev1</t>
+  </si>
+  <si>
+    <t>Activité économique, Production de logements</t>
+  </si>
+  <si>
+    <t>Chiffre d'affaires des entreprises de construction, typologie des constructions</t>
+  </si>
+  <si>
+    <t>À préciser</t>
+  </si>
+  <si>
+    <t>Indicateur économique, ne capture pas directement la qualité de l'habitat</t>
+  </si>
+  <si>
+    <t>https://www.ansd.sn/Indicateur/indice-du-chiffre-daffaires-dans-la-construction-icac</t>
+  </si>
+  <si>
+    <t>A dynamic analysis of winners and losers in Africa's urban housing markets</t>
+  </si>
+  <si>
+    <t>Diana Mitlin et al.</t>
+  </si>
+  <si>
+    <t>ResearchGate</t>
+  </si>
+  <si>
+    <t>Analyse dynamique comparative</t>
+  </si>
+  <si>
+    <t>Analyse des marchés du logement urbain en Afrique (inclut potentiellement le Sénégal)</t>
+  </si>
+  <si>
+    <t>Marchés urbains, Dynamiques socio-économiques</t>
+  </si>
+  <si>
+    <t>Variables à identifier</t>
+  </si>
+  <si>
+    <t>Étude récente, contenu non accessible</t>
+  </si>
+  <si>
+    <t>https://www.researchgate.net/publication/393613303_A_dynamic_analysis_of_winners_and_losers_in_Africa's_urban_housing_markets</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -289,6 +515,14 @@
     <font>
       <b/>
       <sz val="18"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -356,7 +590,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1" indent="1"/>
@@ -391,6 +625,21 @@
     </xf>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="17" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -779,9 +1028,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0ECECF98-72F8-484A-8735-254DB868E3C4}">
   <dimension ref="A1:Q45"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I6" sqref="I6"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A4" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K4" sqref="K4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -1135,4 +1384,413 @@
     <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4B300522-7973-41B7-836A-AE6129584B17}">
+  <dimension ref="A1:K11"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="K3" sqref="K3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
+  <sheetData>
+    <row r="1" spans="1:11" ht="42.75" x14ac:dyDescent="0.45">
+      <c r="A1" s="13" t="s">
+        <v>64</v>
+      </c>
+      <c r="B1" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="13" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="13" t="s">
+        <v>3</v>
+      </c>
+      <c r="E1" s="13" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" s="13" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" s="13" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" s="13" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:11" ht="356.25" x14ac:dyDescent="0.45">
+      <c r="A2" s="14" t="s">
+        <v>11</v>
+      </c>
+      <c r="B2" s="14" t="s">
+        <v>12</v>
+      </c>
+      <c r="C2" s="14">
+        <v>2021</v>
+      </c>
+      <c r="D2" s="14" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" s="14" t="s">
+        <v>65</v>
+      </c>
+      <c r="G2" s="14" t="s">
+        <v>66</v>
+      </c>
+      <c r="H2" s="14" t="s">
+        <v>67</v>
+      </c>
+      <c r="I2" s="14" t="s">
+        <v>68</v>
+      </c>
+      <c r="J2" s="14" t="s">
+        <v>69</v>
+      </c>
+      <c r="K2" s="15" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="342" x14ac:dyDescent="0.45">
+      <c r="A3" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="B3" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="14">
+        <v>2021</v>
+      </c>
+      <c r="D3" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="E3" s="14" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="14" t="s">
+        <v>71</v>
+      </c>
+      <c r="G3" s="14" t="s">
+        <v>26</v>
+      </c>
+      <c r="H3" s="14" t="s">
+        <v>72</v>
+      </c>
+      <c r="I3" s="14" t="s">
+        <v>28</v>
+      </c>
+      <c r="J3" s="14" t="s">
+        <v>73</v>
+      </c>
+      <c r="K3" s="15" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="256.5" x14ac:dyDescent="0.45">
+      <c r="A4" s="14" t="s">
+        <v>32</v>
+      </c>
+      <c r="B4" s="14" t="s">
+        <v>33</v>
+      </c>
+      <c r="C4" s="14" t="s">
+        <v>74</v>
+      </c>
+      <c r="D4" s="14" t="s">
+        <v>75</v>
+      </c>
+      <c r="E4" s="14" t="s">
+        <v>76</v>
+      </c>
+      <c r="F4" s="14" t="s">
+        <v>77</v>
+      </c>
+      <c r="G4" s="14" t="s">
+        <v>36</v>
+      </c>
+      <c r="H4" s="14" t="s">
+        <v>78</v>
+      </c>
+      <c r="I4" s="14" t="s">
+        <v>79</v>
+      </c>
+      <c r="J4" s="14" t="s">
+        <v>80</v>
+      </c>
+      <c r="K4" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="285" x14ac:dyDescent="0.45">
+      <c r="A5" s="14" t="s">
+        <v>81</v>
+      </c>
+      <c r="B5" s="14" t="s">
+        <v>82</v>
+      </c>
+      <c r="C5" s="14">
+        <v>2013</v>
+      </c>
+      <c r="D5" s="14" t="s">
+        <v>83</v>
+      </c>
+      <c r="E5" s="14" t="s">
+        <v>84</v>
+      </c>
+      <c r="F5" s="14" t="s">
+        <v>85</v>
+      </c>
+      <c r="G5" s="14" t="s">
+        <v>44</v>
+      </c>
+      <c r="H5" s="14" t="s">
+        <v>86</v>
+      </c>
+      <c r="I5" s="16">
+        <v>41426</v>
+      </c>
+      <c r="J5" s="14" t="s">
+        <v>87</v>
+      </c>
+      <c r="K5" s="14" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="285" x14ac:dyDescent="0.45">
+      <c r="A6" s="14" t="s">
+        <v>49</v>
+      </c>
+      <c r="B6" s="14" t="s">
+        <v>50</v>
+      </c>
+      <c r="C6" s="14">
+        <v>1996</v>
+      </c>
+      <c r="D6" s="14" t="s">
+        <v>88</v>
+      </c>
+      <c r="E6" s="14" t="s">
+        <v>89</v>
+      </c>
+      <c r="F6" s="14" t="s">
+        <v>90</v>
+      </c>
+      <c r="G6" s="14" t="s">
+        <v>91</v>
+      </c>
+      <c r="H6" s="14" t="s">
+        <v>92</v>
+      </c>
+      <c r="I6" s="14" t="s">
+        <v>93</v>
+      </c>
+      <c r="J6" s="14" t="s">
+        <v>94</v>
+      </c>
+      <c r="K6" s="14" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="356.25" x14ac:dyDescent="0.45">
+      <c r="A7" s="14" t="s">
+        <v>96</v>
+      </c>
+      <c r="B7" s="14" t="s">
+        <v>97</v>
+      </c>
+      <c r="C7" s="14">
+        <v>2013</v>
+      </c>
+      <c r="D7" s="14" t="s">
+        <v>98</v>
+      </c>
+      <c r="E7" s="14" t="s">
+        <v>99</v>
+      </c>
+      <c r="F7" s="14" t="s">
+        <v>100</v>
+      </c>
+      <c r="G7" s="14" t="s">
+        <v>101</v>
+      </c>
+      <c r="H7" s="14" t="s">
+        <v>102</v>
+      </c>
+      <c r="I7" s="16">
+        <v>41456</v>
+      </c>
+      <c r="J7" s="14" t="s">
+        <v>103</v>
+      </c>
+      <c r="K7" s="15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" ht="171" x14ac:dyDescent="0.45">
+      <c r="A8" s="14" t="s">
+        <v>105</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C8" s="14">
+        <v>2013</v>
+      </c>
+      <c r="D8" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>108</v>
+      </c>
+      <c r="F8" s="14" t="s">
+        <v>109</v>
+      </c>
+      <c r="G8" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="H8" s="14" t="s">
+        <v>111</v>
+      </c>
+      <c r="I8" s="14">
+        <v>2013</v>
+      </c>
+      <c r="J8" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="K8" s="15" t="s">
+        <v>113</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" ht="156.75" x14ac:dyDescent="0.45">
+      <c r="A9" s="14" t="s">
+        <v>114</v>
+      </c>
+      <c r="B9" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C9" s="14">
+        <v>2018</v>
+      </c>
+      <c r="D9" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E9" s="14" t="s">
+        <v>115</v>
+      </c>
+      <c r="F9" s="14" t="s">
+        <v>116</v>
+      </c>
+      <c r="G9" s="14" t="s">
+        <v>117</v>
+      </c>
+      <c r="H9" s="14" t="s">
+        <v>118</v>
+      </c>
+      <c r="I9" s="14">
+        <v>2018</v>
+      </c>
+      <c r="J9" s="14" t="s">
+        <v>119</v>
+      </c>
+      <c r="K9" s="15" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" ht="142.5" x14ac:dyDescent="0.45">
+      <c r="A10" s="14" t="s">
+        <v>121</v>
+      </c>
+      <c r="B10" s="14" t="s">
+        <v>106</v>
+      </c>
+      <c r="C10" s="17" t="s">
+        <v>122</v>
+      </c>
+      <c r="D10" s="14" t="s">
+        <v>107</v>
+      </c>
+      <c r="E10" s="14" t="s">
+        <v>123</v>
+      </c>
+      <c r="F10" s="14" t="s">
+        <v>124</v>
+      </c>
+      <c r="G10" s="14" t="s">
+        <v>125</v>
+      </c>
+      <c r="H10" s="14" t="s">
+        <v>126</v>
+      </c>
+      <c r="I10" s="17" t="s">
+        <v>127</v>
+      </c>
+      <c r="J10" s="14" t="s">
+        <v>128</v>
+      </c>
+      <c r="K10" s="15" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" ht="171" x14ac:dyDescent="0.45">
+      <c r="A11" s="14" t="s">
+        <v>130</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>131</v>
+      </c>
+      <c r="C11" s="14">
+        <v>2025</v>
+      </c>
+      <c r="D11" s="14" t="s">
+        <v>132</v>
+      </c>
+      <c r="E11" s="14" t="s">
+        <v>133</v>
+      </c>
+      <c r="F11" s="14" t="s">
+        <v>134</v>
+      </c>
+      <c r="G11" s="14" t="s">
+        <v>135</v>
+      </c>
+      <c r="H11" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="I11" s="16">
+        <v>45778</v>
+      </c>
+      <c r="J11" s="14" t="s">
+        <v>137</v>
+      </c>
+      <c r="K11" s="15" t="s">
+        <v>138</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="K2" r:id="rId1" xr:uid="{C5036F22-4AFB-4E85-8FC9-17DD28845B02}"/>
+    <hyperlink ref="K3" r:id="rId2" xr:uid="{9DC64AA6-24B5-464D-B043-55B4A39B5B0B}"/>
+    <hyperlink ref="K7" r:id="rId3" xr:uid="{752EA32D-43E5-4E14-A132-7DDBA122B197}"/>
+    <hyperlink ref="K8" r:id="rId4" xr:uid="{1AE570CB-0EF1-41B7-A218-0179135C9E6D}"/>
+    <hyperlink ref="K9" r:id="rId5" xr:uid="{89152EFB-6EB2-4488-9D65-D8C76DD793C8}"/>
+    <hyperlink ref="K10" r:id="rId6" xr:uid="{170DA768-6D27-4E38-A66B-48E19A83DEF3}"/>
+    <hyperlink ref="K11" r:id="rId7" xr:uid="{962445E7-FA8A-49F9-A439-2ED39644F849}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>